<commit_message>
update with 3 selection options en extra boodschappen
</commit_message>
<xml_diff>
--- a/data-raw/data/recepten.xlsx
+++ b/data-raw/data/recepten.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eekhouti\Documents\GitHub\wisselmenu\data-raw\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E50A92E-D6E3-418F-BB9F-150CBFB943B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D195A8-D08A-4050-9506-73C3D9880A40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DEE8369E-45A2-425F-AF40-529136F4C573}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9108" xr2:uid="{DEE8369E-45A2-425F-AF40-529136F4C573}"/>
   </bookViews>
   <sheets>
     <sheet name="recepten" sheetId="1" r:id="rId1"/>
-    <sheet name="producten" sheetId="2" r:id="rId2"/>
+    <sheet name="boodschappen" sheetId="3" r:id="rId2"/>
+    <sheet name="producten" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Extract" localSheetId="1">producten!$A:$A</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="2">producten!$A:$A</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="165">
   <si>
     <t>genre</t>
   </si>
@@ -430,6 +431,108 @@
   </si>
   <si>
     <t>noten</t>
+  </si>
+  <si>
+    <t>producten</t>
+  </si>
+  <si>
+    <t>aantal</t>
+  </si>
+  <si>
+    <t>appels</t>
+  </si>
+  <si>
+    <t>bananen</t>
+  </si>
+  <si>
+    <t>kiwi's</t>
+  </si>
+  <si>
+    <t>peren</t>
+  </si>
+  <si>
+    <t>brood</t>
+  </si>
+  <si>
+    <t>volkoren brood</t>
+  </si>
+  <si>
+    <t>afbak broodjes</t>
+  </si>
+  <si>
+    <t>huishoud</t>
+  </si>
+  <si>
+    <t>wc papier</t>
+  </si>
+  <si>
+    <t>vochtig toiletpapier</t>
+  </si>
+  <si>
+    <t>toiletblokjes</t>
+  </si>
+  <si>
+    <t>allesreiniger</t>
+  </si>
+  <si>
+    <t>dolce gusto lungo</t>
+  </si>
+  <si>
+    <t>dolce gusto grande</t>
+  </si>
+  <si>
+    <t>dolce gusto</t>
+  </si>
+  <si>
+    <t>koffiethee</t>
+  </si>
+  <si>
+    <t>vleeswaren</t>
+  </si>
+  <si>
+    <t>boterhamworst</t>
+  </si>
+  <si>
+    <t>gerookte kip</t>
+  </si>
+  <si>
+    <t>hummus</t>
+  </si>
+  <si>
+    <t>ontbijt</t>
+  </si>
+  <si>
+    <t>cracottes</t>
+  </si>
+  <si>
+    <t>ontbijtcrackers</t>
+  </si>
+  <si>
+    <t>jam</t>
+  </si>
+  <si>
+    <t>volkoren beschuit</t>
+  </si>
+  <si>
+    <t>cruesly</t>
+  </si>
+  <si>
+    <t>cornflakes</t>
+  </si>
+  <si>
+    <t>melk</t>
+  </si>
+  <si>
+    <t>vla</t>
+  </si>
+  <si>
+    <t>boter</t>
+  </si>
+  <si>
+    <t>kaas (30+)</t>
+  </si>
+  <si>
+    <t>eieren</t>
   </si>
 </sst>
 </file>
@@ -789,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129ED249-F640-46C9-8763-FFC59B9BA506}">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -967,6 +1070,9 @@
       <c r="G8">
         <v>25</v>
       </c>
+      <c r="H8">
+        <v>450</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1061,11 +1167,11 @@
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="D13">
-        <v>1</v>
+      <c r="D13" t="s">
+        <v>87</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>164</v>
       </c>
       <c r="G13">
         <v>25</v>
@@ -1359,6 +1465,12 @@
       <c r="B27" t="s">
         <v>35</v>
       </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>103</v>
+      </c>
       <c r="F27" t="s">
         <v>36</v>
       </c>
@@ -1798,7 +1910,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -1814,8 +1926,14 @@
       <c r="F49" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <v>20</v>
+      </c>
+      <c r="H49">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1831,8 +1949,14 @@
       <c r="F50" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <v>20</v>
+      </c>
+      <c r="H50">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -1848,8 +1972,14 @@
       <c r="F51" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51">
+        <v>20</v>
+      </c>
+      <c r="H51">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -1865,8 +1995,14 @@
       <c r="F52" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52">
+        <v>20</v>
+      </c>
+      <c r="H52">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -1882,8 +2018,14 @@
       <c r="F53" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53">
+        <v>20</v>
+      </c>
+      <c r="H53">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -1896,8 +2038,11 @@
       <c r="F54" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>42</v>
       </c>
@@ -1913,8 +2058,11 @@
       <c r="F55" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>42</v>
       </c>
@@ -1930,8 +2078,11 @@
       <c r="F56" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G56">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>42</v>
       </c>
@@ -1947,8 +2098,11 @@
       <c r="F57" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -1964,8 +2118,11 @@
       <c r="F58" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>42</v>
       </c>
@@ -1975,8 +2132,11 @@
       <c r="F59" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G59">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>42</v>
       </c>
@@ -1986,8 +2146,11 @@
       <c r="F60" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G60">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>34</v>
       </c>
@@ -2003,8 +2166,11 @@
       <c r="F61" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G61">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -2014,8 +2180,11 @@
       <c r="F62" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G62">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>34</v>
       </c>
@@ -2028,8 +2197,11 @@
       <c r="F63" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>34</v>
       </c>
@@ -2044,6 +2216,9 @@
       </c>
       <c r="F64" t="s">
         <v>39</v>
+      </c>
+      <c r="G64">
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
@@ -2059,6 +2234,9 @@
       <c r="F65" t="s">
         <v>82</v>
       </c>
+      <c r="G65">
+        <v>15</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
@@ -2070,6 +2248,9 @@
       <c r="F66" t="s">
         <v>70</v>
       </c>
+      <c r="G66">
+        <v>15</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
@@ -2451,7 +2632,7 @@
         <v>35</v>
       </c>
       <c r="E82" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F82" t="s">
         <v>47</v>
@@ -2499,6 +2680,9 @@
       <c r="F84" t="s">
         <v>14</v>
       </c>
+      <c r="G84">
+        <v>30</v>
+      </c>
       <c r="H84">
         <v>450</v>
       </c>
@@ -2522,6 +2706,9 @@
       <c r="F85" t="s">
         <v>101</v>
       </c>
+      <c r="G85">
+        <v>30</v>
+      </c>
       <c r="H85">
         <v>450</v>
       </c>
@@ -2542,6 +2729,9 @@
       <c r="F86" t="s">
         <v>90</v>
       </c>
+      <c r="G86">
+        <v>30</v>
+      </c>
       <c r="H86">
         <v>450</v>
       </c>
@@ -2565,6 +2755,9 @@
       <c r="F87" t="s">
         <v>102</v>
       </c>
+      <c r="G87">
+        <v>30</v>
+      </c>
       <c r="H87">
         <v>450</v>
       </c>
@@ -2585,6 +2778,9 @@
       <c r="F88" t="s">
         <v>69</v>
       </c>
+      <c r="G88">
+        <v>30</v>
+      </c>
       <c r="H88">
         <v>450</v>
       </c>
@@ -2605,6 +2801,9 @@
       <c r="F89" t="s">
         <v>37</v>
       </c>
+      <c r="G89">
+        <v>30</v>
+      </c>
       <c r="H89">
         <v>450</v>
       </c>
@@ -2628,6 +2827,9 @@
       <c r="F90" t="s">
         <v>104</v>
       </c>
+      <c r="G90">
+        <v>30</v>
+      </c>
       <c r="H90">
         <v>450</v>
       </c>
@@ -2651,6 +2853,9 @@
       <c r="F91" t="s">
         <v>47</v>
       </c>
+      <c r="G91">
+        <v>30</v>
+      </c>
       <c r="H91">
         <v>450</v>
       </c>
@@ -2671,6 +2876,9 @@
       <c r="F92" t="s">
         <v>106</v>
       </c>
+      <c r="G92">
+        <v>30</v>
+      </c>
       <c r="H92">
         <v>450</v>
       </c>
@@ -2694,6 +2902,9 @@
       <c r="F93" t="s">
         <v>12</v>
       </c>
+      <c r="G93">
+        <v>30</v>
+      </c>
       <c r="H93">
         <v>450</v>
       </c>
@@ -2717,6 +2928,9 @@
       <c r="F94" t="s">
         <v>107</v>
       </c>
+      <c r="G94">
+        <v>30</v>
+      </c>
       <c r="H94">
         <v>450</v>
       </c>
@@ -2734,6 +2948,9 @@
       <c r="F95" t="s">
         <v>108</v>
       </c>
+      <c r="G95">
+        <v>30</v>
+      </c>
       <c r="H95">
         <v>450</v>
       </c>
@@ -2754,6 +2971,9 @@
       <c r="F96" t="s">
         <v>109</v>
       </c>
+      <c r="G96">
+        <v>30</v>
+      </c>
       <c r="H96">
         <v>450</v>
       </c>
@@ -2777,6 +2997,9 @@
       <c r="F97" t="s">
         <v>112</v>
       </c>
+      <c r="G97">
+        <v>20</v>
+      </c>
       <c r="H97">
         <v>470</v>
       </c>
@@ -2800,6 +3023,9 @@
       <c r="F98" t="s">
         <v>113</v>
       </c>
+      <c r="G98">
+        <v>20</v>
+      </c>
       <c r="H98">
         <v>470</v>
       </c>
@@ -2823,6 +3049,9 @@
       <c r="F99" t="s">
         <v>23</v>
       </c>
+      <c r="G99">
+        <v>20</v>
+      </c>
       <c r="H99">
         <v>470</v>
       </c>
@@ -2846,6 +3075,9 @@
       <c r="F100" t="s">
         <v>36</v>
       </c>
+      <c r="G100">
+        <v>20</v>
+      </c>
       <c r="H100">
         <v>470</v>
       </c>
@@ -2866,6 +3098,9 @@
       <c r="F101" t="s">
         <v>77</v>
       </c>
+      <c r="G101">
+        <v>20</v>
+      </c>
       <c r="H101">
         <v>470</v>
       </c>
@@ -2886,6 +3121,9 @@
       <c r="F102" t="s">
         <v>114</v>
       </c>
+      <c r="G102">
+        <v>20</v>
+      </c>
       <c r="H102">
         <v>470</v>
       </c>
@@ -2906,6 +3144,9 @@
       <c r="F103" t="s">
         <v>34</v>
       </c>
+      <c r="G103">
+        <v>20</v>
+      </c>
       <c r="H103">
         <v>470</v>
       </c>
@@ -2929,6 +3170,9 @@
       <c r="F104" t="s">
         <v>39</v>
       </c>
+      <c r="G104">
+        <v>20</v>
+      </c>
       <c r="H104">
         <v>470</v>
       </c>
@@ -2952,6 +3196,9 @@
       <c r="F105" t="s">
         <v>54</v>
       </c>
+      <c r="G105">
+        <v>30</v>
+      </c>
       <c r="H105">
         <v>480</v>
       </c>
@@ -2972,6 +3219,9 @@
       <c r="F106" t="s">
         <v>117</v>
       </c>
+      <c r="G106">
+        <v>30</v>
+      </c>
       <c r="H106">
         <v>480</v>
       </c>
@@ -2992,6 +3242,9 @@
       <c r="F107" t="s">
         <v>114</v>
       </c>
+      <c r="G107">
+        <v>30</v>
+      </c>
       <c r="H107">
         <v>480</v>
       </c>
@@ -3012,6 +3265,9 @@
       <c r="F108" t="s">
         <v>90</v>
       </c>
+      <c r="G108">
+        <v>30</v>
+      </c>
       <c r="H108">
         <v>480</v>
       </c>
@@ -3035,6 +3291,9 @@
       <c r="F109" t="s">
         <v>118</v>
       </c>
+      <c r="G109">
+        <v>30</v>
+      </c>
       <c r="H109">
         <v>480</v>
       </c>
@@ -3058,6 +3317,9 @@
       <c r="F110" t="s">
         <v>119</v>
       </c>
+      <c r="G110">
+        <v>30</v>
+      </c>
       <c r="H110">
         <v>480</v>
       </c>
@@ -3081,6 +3343,9 @@
       <c r="F111" t="s">
         <v>120</v>
       </c>
+      <c r="G111">
+        <v>30</v>
+      </c>
       <c r="H111">
         <v>480</v>
       </c>
@@ -3104,6 +3369,9 @@
       <c r="F112" t="s">
         <v>121</v>
       </c>
+      <c r="G112">
+        <v>30</v>
+      </c>
       <c r="H112">
         <v>480</v>
       </c>
@@ -3126,6 +3394,9 @@
       </c>
       <c r="F113" t="s">
         <v>23</v>
+      </c>
+      <c r="G113">
+        <v>30</v>
       </c>
       <c r="H113">
         <v>480</v>
@@ -3138,11 +3409,272 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8E668A-EF38-46AB-BBE2-219F259C8063}">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>153</v>
+      </c>
+      <c r="D22" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>126</v>
+      </c>
+      <c r="D29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A483436E-7523-47A0-B77D-347D7F578864}">
   <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>